<commit_message>
abiotic factor data entry
</commit_message>
<xml_diff>
--- a/GC-Data-Raw-R/GC-Data-standardizedfilenames/runsheets-standardizedfilenames/runsheet_20140114_V.xlsx
+++ b/GC-Data-Raw-R/GC-Data-standardizedfilenames/runsheets-standardizedfilenames/runsheet_20140114_V.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="19020" yWindow="0" windowWidth="14180" windowHeight="17820" tabRatio="500"/>
@@ -210,66 +210,6 @@
     <t>F3-E-17-T30</t>
   </si>
   <si>
-    <t>F2-A-17-T0</t>
-  </si>
-  <si>
-    <t>F2-A-17-T10</t>
-  </si>
-  <si>
-    <t>F2-A-17-T20</t>
-  </si>
-  <si>
-    <t>F2-A-17-T30</t>
-  </si>
-  <si>
-    <t>F2-B-17-T0</t>
-  </si>
-  <si>
-    <t>F2-B-17-T10</t>
-  </si>
-  <si>
-    <t>F2-B-17-T20</t>
-  </si>
-  <si>
-    <t>F2-B-17-T30</t>
-  </si>
-  <si>
-    <t>F2-C-17-T0</t>
-  </si>
-  <si>
-    <t>F2-C-17-T10</t>
-  </si>
-  <si>
-    <t>F2-C-17-T20</t>
-  </si>
-  <si>
-    <t>F2-C-17-T30</t>
-  </si>
-  <si>
-    <t>F2-D-17-T0</t>
-  </si>
-  <si>
-    <t>F2-D-17-T10</t>
-  </si>
-  <si>
-    <t>F2-D-17-T20</t>
-  </si>
-  <si>
-    <t>F2-D-17-T30</t>
-  </si>
-  <si>
-    <t>F2-E-17-T0</t>
-  </si>
-  <si>
-    <t>F2-E-17-T10</t>
-  </si>
-  <si>
-    <t>F2-E-17-T20</t>
-  </si>
-  <si>
-    <t>F2-E-17-T30</t>
-  </si>
-  <si>
     <t>S1-A-18-T0</t>
   </si>
   <si>
@@ -331,6 +271,66 @@
   </si>
   <si>
     <t>2013.12.18</t>
+  </si>
+  <si>
+    <t>F1-A-17-T0</t>
+  </si>
+  <si>
+    <t>F1-A-17-T10</t>
+  </si>
+  <si>
+    <t>F1-A-17-T20</t>
+  </si>
+  <si>
+    <t>F1-A-17-T30</t>
+  </si>
+  <si>
+    <t>F1-B-17-T0</t>
+  </si>
+  <si>
+    <t>F1-B-17-T10</t>
+  </si>
+  <si>
+    <t>F1-B-17-T20</t>
+  </si>
+  <si>
+    <t>F1-B-17-T30</t>
+  </si>
+  <si>
+    <t>F1-C-17-T0</t>
+  </si>
+  <si>
+    <t>F1-C-17-T10</t>
+  </si>
+  <si>
+    <t>F1-C-17-T20</t>
+  </si>
+  <si>
+    <t>F1-C-17-T30</t>
+  </si>
+  <si>
+    <t>F1-D-17-T0</t>
+  </si>
+  <si>
+    <t>F1-D-17-T10</t>
+  </si>
+  <si>
+    <t>F1-D-17-T20</t>
+  </si>
+  <si>
+    <t>F1-D-17-T30</t>
+  </si>
+  <si>
+    <t>F1-E-17-T0</t>
+  </si>
+  <si>
+    <t>F1-E-17-T10</t>
+  </si>
+  <si>
+    <t>F1-E-17-T20</t>
+  </si>
+  <si>
+    <t>F1-E-17-T30</t>
   </si>
 </sst>
 </file>
@@ -1241,8 +1241,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3098,11 +3098,11 @@
         <v>21</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>63</v>
+        <v>84</v>
       </c>
       <c r="F52" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -3135,11 +3135,11 @@
         <v>21</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>64</v>
+        <v>85</v>
       </c>
       <c r="F53" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -3172,11 +3172,11 @@
         <v>21</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="F54" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -3209,11 +3209,11 @@
         <v>21</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="F55" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -3246,11 +3246,11 @@
         <v>21</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="F56" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G56" t="str">
         <f t="shared" si="1"/>
@@ -3283,11 +3283,11 @@
         <v>21</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="F57" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -3320,11 +3320,11 @@
         <v>21</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="F58" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -3357,11 +3357,11 @@
         <v>21</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="F59" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="1"/>
@@ -3394,11 +3394,11 @@
         <v>21</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="F60" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -3431,11 +3431,11 @@
         <v>21</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="F61" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -3468,11 +3468,11 @@
         <v>21</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="F62" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -3505,11 +3505,11 @@
         <v>21</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="F63" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -3542,11 +3542,11 @@
         <v>21</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="F64" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -3579,11 +3579,11 @@
         <v>21</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="F65" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -3616,11 +3616,11 @@
         <v>21</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="F66" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="1"/>
@@ -3653,11 +3653,11 @@
         <v>21</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="F67" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="1"/>
@@ -3690,11 +3690,11 @@
         <v>21</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="F68" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
@@ -3727,11 +3727,11 @@
         <v>21</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="F69" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
@@ -3764,11 +3764,11 @@
         <v>21</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="F70" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
@@ -3801,11 +3801,11 @@
         <v>21</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="F71" t="str">
         <f t="shared" si="0"/>
-        <v>F2</v>
+        <v>F1</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
@@ -3835,10 +3835,10 @@
         <v>10</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="F72" t="str">
         <f t="shared" si="0"/>
@@ -3872,10 +3872,10 @@
         <v>10</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="F73" t="str">
         <f t="shared" si="0"/>
@@ -3909,10 +3909,10 @@
         <v>10</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="F74" t="str">
         <f t="shared" si="0"/>
@@ -3946,10 +3946,10 @@
         <v>10</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="F75" t="str">
         <f t="shared" si="0"/>
@@ -3983,10 +3983,10 @@
         <v>10</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="F76" t="str">
         <f t="shared" ref="F76:F91" si="5">LEFT(E76,2)</f>
@@ -4020,10 +4020,10 @@
         <v>42</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="F77" t="str">
         <f t="shared" si="5"/>
@@ -4057,10 +4057,10 @@
         <v>10</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="F78" t="str">
         <f t="shared" si="5"/>
@@ -4094,10 +4094,10 @@
         <v>42</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F79" t="str">
         <f t="shared" si="5"/>
@@ -4131,10 +4131,10 @@
         <v>10</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="F80" t="str">
         <f t="shared" si="5"/>
@@ -4168,10 +4168,10 @@
         <v>10</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="F81" t="str">
         <f t="shared" si="5"/>
@@ -4205,10 +4205,10 @@
         <v>10</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="F82" t="str">
         <f t="shared" si="5"/>
@@ -4242,10 +4242,10 @@
         <v>10</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="F83" t="str">
         <f t="shared" si="5"/>
@@ -4279,10 +4279,10 @@
         <v>10</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="F84" t="str">
         <f t="shared" si="5"/>
@@ -4316,10 +4316,10 @@
         <v>10</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F85" t="str">
         <f t="shared" si="5"/>
@@ -4353,10 +4353,10 @@
         <v>10</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="F86" t="str">
         <f t="shared" si="5"/>
@@ -4390,10 +4390,10 @@
         <v>10</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="F87" t="str">
         <f t="shared" si="5"/>
@@ -4427,10 +4427,10 @@
         <v>10</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="F88" t="str">
         <f t="shared" si="5"/>
@@ -4464,10 +4464,10 @@
         <v>10</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="F89" t="str">
         <f t="shared" si="5"/>
@@ -4501,10 +4501,10 @@
         <v>10</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="F90" t="str">
         <f t="shared" si="5"/>
@@ -4538,10 +4538,10 @@
         <v>10</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="F91" t="str">
         <f t="shared" si="5"/>

</xml_diff>